<commit_message>
Implemented new code as per below approach: One Excel per feature, One row per scenario, Cross-scenario data reuse, Runtime + persisted storage, Zero hard-coding, Scales to regression suites
</commit_message>
<xml_diff>
--- a/cucumber-for-appian/src/test/resources/testdata/TestData.xlsx
+++ b/cucumber-for-appian/src/test/resources/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ORIXAutomatedTest\cucumber-for-appian\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\ORIXAutoExcel\cucumber-for-appian\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0AE195-8E1D-4496-9838-EF2177804AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A450984F-4370-4A16-B45E-A71339261EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="873" firstSheet="3" activeTab="7" xr2:uid="{25A2403C-A232-4567-AEA7-838C07E97658}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="873" firstSheet="3" activeTab="8" xr2:uid="{25A2403C-A232-4567-AEA7-838C07E97658}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="169">
   <si>
     <t>FieldName</t>
   </si>
@@ -505,16 +505,6 @@
     <t>Deposit Amount[3]</t>
   </si>
   <si>
-    <t>APP-436</t>
-  </si>
-  <si>
-    <t>SMB-00000655
-SMB-00000655</t>
-  </si>
-  <si>
-    <t>11 Dec 2025 07:26 PM</t>
-  </si>
-  <si>
     <t>Take Ownership</t>
   </si>
   <si>
@@ -555,26 +545,6 @@
   </si>
   <si>
     <t>Equifax Check</t>
-  </si>
-  <si>
-    <t>APP-438</t>
-  </si>
-  <si>
-    <t>SMB-00000657
-SMB-00000657</t>
-  </si>
-  <si>
-    <t>11 Dec 2025 11:04 PM</t>
-  </si>
-  <si>
-    <t>APP-439</t>
-  </si>
-  <si>
-    <t>SMB-00000658
-SMB-00000658</t>
-  </si>
-  <si>
-    <t>11 Dec 2025 11:14 PM</t>
   </si>
   <si>
     <t>APP-440</t>
@@ -591,7 +561,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -987,15 +956,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.109375"/>
-    <col min="2" max="2" customWidth="true" width="61.77734375"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="61.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1018,31 +987,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.33203125"/>
-    <col min="2" max="2" customWidth="true" width="71.77734375"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="71.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1061,63 +1030,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0"/>
-    <col min="2" max="2" customWidth="true" width="34.6640625"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>175</v>
+      <c r="B2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>176</v>
+      <c r="B3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>177</v>
+      <c r="B6" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1136,31 +1105,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.5546875"/>
-    <col min="2" max="2" customWidth="true" width="63.6640625"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1179,46 +1148,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.21875"/>
-    <col min="2" max="2" customWidth="true" width="55.109375"/>
-    <col min="4" max="4" customWidth="true" width="26.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="1" max="1" width="40.21875" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1226,31 +1195,31 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>71</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1258,112 +1227,112 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>76</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>80</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>88310877</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>68173780899</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>68173780899</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1392,23 +1361,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.109375"/>
-    <col min="2" max="2" customWidth="true" width="18.109375"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1427,87 +1396,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.33203125"/>
-    <col min="2" max="2" customWidth="true" width="71.77734375"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="71.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1526,191 +1495,191 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.77734375"/>
-    <col min="2" max="2" customWidth="true" width="38.44140625"/>
+    <col min="1" max="1" width="44.77734375" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>150</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>151</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>85</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>91</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>93</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>94</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s" s="0">
+      <c r="A14" t="s">
         <v>96</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s" s="0">
+      <c r="A15" t="s">
         <v>98</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
         <v>100</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
         <v>102</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s" s="0">
+      <c r="A18" t="s">
         <v>104</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="B18" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s" s="0">
+      <c r="A19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="B19" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s" s="0">
+      <c r="A20" t="s">
         <v>107</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="B20" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s" s="0">
+      <c r="A21" t="s">
         <v>109</v>
       </c>
-      <c r="B21" t="s" s="0">
+      <c r="B21" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" t="s" s="0">
+      <c r="A22" t="s">
         <v>111</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B22" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" t="s" s="0">
+      <c r="A23" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="0">
+      <c r="B23">
         <v>2.68</v>
       </c>
     </row>
@@ -1729,71 +1698,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0"/>
-    <col min="2" max="2" customWidth="true" width="34.6640625"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1806,118 +1775,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE54915-588F-4484-B362-119D2933340A}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.6640625"/>
-    <col min="2" max="2" customWidth="true" width="29.21875"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>118</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>121</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>124</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>126</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>127</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>155</v>
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s" s="0">
-        <v>156</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>156</v>
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>157</v>
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s" s="0">
-        <v>168</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>167</v>
+      <c r="A13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1930,150 +1899,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59ADD8AA-201A-4DDB-A594-636647615EA5}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.88671875"/>
-    <col min="2" max="2" customWidth="true" width="43.5546875"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="43.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>107</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>133</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>134</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>136</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>138</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>140</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>142</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>143</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>145</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>147</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>102</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
         <v>158</v>
       </c>
-      <c r="B13" t="s" s="0">
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s" s="0">
+      <c r="B15" t="s">
         <v>160</v>
       </c>
-      <c r="B14" t="s" s="0">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s" s="0">
+      <c r="B16" t="s">
         <v>162</v>
       </c>
-      <c r="B15" t="s" s="0">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s" s="0">
-        <v>166</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>165</v>
+      <c r="B17" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>